<commit_message>
Test Mobile + Web Landing
</commit_message>
<xml_diff>
--- a/Docs/Landing_Offline/LandingOffline.xlsx
+++ b/Docs/Landing_Offline/LandingOffline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c01515023adb62f/Desktop/Talent/TalentTechDocs/Docs/Landing_Offline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Desktop\Talent\TalentTechDocs\Docs\Landing_Offline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{279348F9-A7D7-4189-BA9A-3E26FB5354C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{68F02445-D500-4CD0-880E-53562211B50A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3242A86-7FA2-474B-8A6C-D1E05A49AFFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>